<commit_message>
Coorect PRJ unique: false
</commit_message>
<xml_diff>
--- a/data/result/validation_errors.xlsx
+++ b/data/result/validation_errors.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -601,7 +601,7 @@
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B7" t="n">
         <v>3</v>
@@ -613,7 +613,7 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>PRJ-999</t>
+          <t>WRONG-FORMAT</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -623,25 +623,25 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Duplicate found: PRJ-999</t>
+          <t>Pattern mismatch</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="B8" t="n">
         <v>3</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>project_code</t>
+          <t>created_at</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>WRONG-FORMAT</t>
+          <t>2027-01-01</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
@@ -651,26 +651,24 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>Pattern mismatch</t>
+          <t>Year later than 2026</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B9" t="n">
         <v>3</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>project_code</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>PRJ-777</t>
-        </is>
+          <t>created_at</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>4654654.23</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
@@ -679,117 +677,7 @@
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>Duplicate found: PRJ-777</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="n">
-        <v>38</v>
-      </c>
-      <c r="B10" t="n">
-        <v>3</v>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>created_at</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>2027-01-01</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>VALIDATION_FAILED</t>
-        </is>
-      </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>Year later than 2026</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="n">
-        <v>39</v>
-      </c>
-      <c r="B11" t="n">
-        <v>3</v>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>project_code</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>PRJ-666</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>VALIDATION_FAILED</t>
-        </is>
-      </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>Duplicate found: PRJ-666</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="n">
-        <v>39</v>
-      </c>
-      <c r="B12" t="n">
-        <v>3</v>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>created_at</t>
-        </is>
-      </c>
-      <c r="D12" t="n">
-        <v>4654654.23</v>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>VALIDATION_FAILED</t>
-        </is>
-      </c>
-      <c r="F12" t="inlineStr">
-        <is>
           <t>Datetime processing failed: cannot convert input with unit 'D'</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="n">
-        <v>41</v>
-      </c>
-      <c r="B13" t="n">
-        <v>3</v>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>project_code</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>PRJ-555</t>
-        </is>
-      </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>VALIDATION_FAILED</t>
-        </is>
-      </c>
-      <c r="F13" t="inlineStr">
-        <is>
-          <t>Duplicate found: PRJ-555</t>
         </is>
       </c>
     </row>

</xml_diff>